<commit_message>
Update doc to fit header generation needs and CLR bit position
</commit_message>
<xml_diff>
--- a/doc/SPI_reference.xlsx
+++ b/doc/SPI_reference.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Info " sheetId="1" state="visible" r:id="rId2"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="338">
   <si>
     <t xml:space="preserve">Document Information</t>
   </si>
@@ -785,7 +785,7 @@
     <t xml:space="preserve">Command name</t>
   </si>
   <si>
-    <t xml:space="preserve">Command Field</t>
+    <t xml:space="preserve">Command field</t>
   </si>
   <si>
     <t xml:space="preserve">Parameter</t>
@@ -905,13 +905,16 @@
     <t xml:space="preserve">Sets size and starts uDMA tx/rx channel</t>
   </si>
   <si>
-    <t xml:space="preserve">Parameter Bit field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Field Value</t>
+    <t xml:space="preserve">Parameter bit field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Field value</t>
   </si>
   <si>
     <t xml:space="preserve">CLKDIV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARG</t>
   </si>
   <si>
     <t xml:space="preserve">Sets the clock divider value</t>
@@ -988,16 +991,10 @@
     <t xml:space="preserve">Select the SPIM command to be processed. Here “DUMMY”</t>
   </si>
   <si>
-    <t xml:space="preserve">EVENT_ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">External event id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CYCLE_COUNT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of wait cycles</t>
+    <t xml:space="preserve">EVENT_ID_CYCLE_COUNT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">External event id or Number of wait cycles</t>
   </si>
   <si>
     <t xml:space="preserve">WAIT_TYPE</t>
@@ -1108,16 +1105,13 @@
     <t xml:space="preserve">START_ADDR</t>
   </si>
   <si>
-    <t xml:space="preserve">L2_AWIDTH_NOAL</t>
-  </si>
-  <si>
     <t xml:space="preserve">L2_AWIDTH_NOAL bits of the starting address</t>
   </si>
   <si>
     <t xml:space="preserve">Select the SPIM command to be processed. Here “SETUP_UCA”</t>
   </si>
   <si>
-    <t xml:space="preserve">TRANS_SIZE</t>
+    <t xml:space="preserve">SIZE</t>
   </si>
   <si>
     <t xml:space="preserve">transfer size-1 in bytes. Max size depends on the TRANS_SIZE parameter</t>
@@ -1891,18 +1885,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:D65536"/>
+  <dimension ref="B1:D1048576"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="39.280612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="10.8010204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="39.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="1" width="10.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2150,7 +2144,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2165,24 +2159,24 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="44" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="44" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="44" width="43.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="44" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="23.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="44" width="43.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="45" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C1" s="45" t="s">
         <v>11</v>
@@ -2191,7 +2185,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2204,19 +2198,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D65536"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="25" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.8469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.0255102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.1224489795918"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="22.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="10.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2548,7 +2542,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2563,18 +2557,18 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="44" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="44" width="44.1428571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="44" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="44" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="44" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.1224489795918"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="44" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="44.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="44" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="44" width="24.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="44" width="13.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="10.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2629,7 +2623,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2642,24 +2636,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:53"/>
+  <dimension ref="A1:AMJ53"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="44" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="14" min="11" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="21" min="16" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="3" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="11" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="16" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="10.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3396,7 +3390,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3411,23 +3405,23 @@
   </sheetPr>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="W1" activeCellId="0" sqref="W1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="36" width="18.765306122449"/>
-    <col collapsed="false" hidden="true" max="2" min="2" style="36" width="0"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="36" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="36" width="4.45408163265306"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="36" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="25" width="39.9591836734694"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="36" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="36" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="36" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="36" width="18.77"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="2" min="2" style="36" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="36" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="36" width="4.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="36" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="25" width="39.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="36" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="36" width="9.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="36" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3802,7 +3796,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3815,25 +3809,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H65536"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="bottomLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="35" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="44" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="44" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="44" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="44" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="44" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="44" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="62" width="73.9744897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="63" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="17.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="44" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="44" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="44" width="16.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="44" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="44" width="12.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="62" width="73.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="63" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4604,7 +4598,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4619,23 +4613,23 @@
   </sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="63" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="63" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="44" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="44" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="44" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="44" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="44" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="62" width="30.6428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="63" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="63" width="18.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="63" width="15.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="44" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="44" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="44" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="44" width="14.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="44" width="11.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="62" width="30.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="63" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4667,7 +4661,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4682,17 +4676,18 @@
   </sheetPr>
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.219387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="44" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="44" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="77.7551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="44" width="17.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="44" width="25.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="77.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4953,7 +4948,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4966,21 +4961,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E52" activeCellId="0" sqref="E52"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="35" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="44" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="44" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="44" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="44" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="77.7551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="25.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="44" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="44" width="20.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="44" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="77.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4991,7 +4986,7 @@
         <v>229</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>207</v>
+        <v>104</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>78</v>
@@ -5017,14 +5012,16 @@
       <c r="D2" s="73" t="n">
         <v>8</v>
       </c>
-      <c r="E2" s="73"/>
+      <c r="E2" s="73" t="s">
+        <v>273</v>
+      </c>
       <c r="F2" s="74" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="75" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B3" s="44" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A2</f>
@@ -5036,14 +5033,16 @@
       <c r="D3" s="44" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="0"/>
+      <c r="E3" s="46" t="s">
+        <v>273</v>
+      </c>
       <c r="F3" s="76" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="75" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B4" s="44" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A2</f>
@@ -5055,14 +5054,16 @@
       <c r="D4" s="44" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="0"/>
+      <c r="E4" s="46" t="s">
+        <v>273</v>
+      </c>
       <c r="F4" s="76" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="77" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B5" s="78" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A2</f>
@@ -5079,12 +5080,12 @@
         <v>0x0</v>
       </c>
       <c r="F5" s="79" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="72" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B6" s="73" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A3</f>
@@ -5100,12 +5101,12 @@
         <v>170</v>
       </c>
       <c r="F6" s="80" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="77" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B7" s="78" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A3</f>
@@ -5122,12 +5123,12 @@
         <v>0x1</v>
       </c>
       <c r="F7" s="79" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="72" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B8" s="73" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A4</f>
@@ -5139,14 +5140,16 @@
       <c r="D8" s="73" t="n">
         <v>16</v>
       </c>
-      <c r="E8" s="73"/>
+      <c r="E8" s="73" t="s">
+        <v>273</v>
+      </c>
       <c r="F8" s="74" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="75" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B9" s="44" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A4</f>
@@ -5158,14 +5161,16 @@
       <c r="D9" s="44" t="n">
         <v>4</v>
       </c>
-      <c r="E9" s="0"/>
+      <c r="E9" s="46" t="s">
+        <v>273</v>
+      </c>
       <c r="F9" s="81" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="75" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B10" s="44" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A4</f>
@@ -5177,14 +5182,16 @@
       <c r="D10" s="44" t="n">
         <v>1</v>
       </c>
-      <c r="E10" s="0"/>
+      <c r="E10" s="46" t="s">
+        <v>273</v>
+      </c>
       <c r="F10" s="81" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="75" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B11" s="44" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A4</f>
@@ -5196,14 +5203,16 @@
       <c r="D11" s="44" t="n">
         <v>1</v>
       </c>
-      <c r="E11" s="0"/>
+      <c r="E11" s="46" t="s">
+        <v>273</v>
+      </c>
       <c r="F11" s="81" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="77" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B12" s="78" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A4</f>
@@ -5220,12 +5229,12 @@
         <v>0x2</v>
       </c>
       <c r="F12" s="79" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="72" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B13" s="73" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A5</f>
@@ -5237,14 +5246,16 @@
       <c r="D13" s="73" t="n">
         <v>5</v>
       </c>
-      <c r="E13" s="73"/>
+      <c r="E13" s="73" t="s">
+        <v>273</v>
+      </c>
       <c r="F13" s="74" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="77" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B14" s="78" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A5</f>
@@ -5261,12 +5272,12 @@
         <v>0x4</v>
       </c>
       <c r="F14" s="79" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="72" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B15" s="73" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A6</f>
@@ -5276,701 +5287,742 @@
         <v>0</v>
       </c>
       <c r="D15" s="73" t="n">
+        <v>7</v>
+      </c>
+      <c r="E15" s="73" t="s">
+        <v>273</v>
+      </c>
+      <c r="F15" s="74" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="75" t="s">
+        <v>298</v>
+      </c>
+      <c r="B16" s="66" t="s">
+        <v>242</v>
+      </c>
+      <c r="C16" s="66" t="n">
+        <v>8</v>
+      </c>
+      <c r="D16" s="66" t="n">
         <v>2</v>
       </c>
-      <c r="E15" s="73"/>
-      <c r="F15" s="74" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="75" t="s">
-        <v>297</v>
-      </c>
-      <c r="B16" s="66" t="str">
+      <c r="E16" s="66" t="s">
+        <v>273</v>
+      </c>
+      <c r="F16" s="76" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="77" t="s">
+        <v>279</v>
+      </c>
+      <c r="B17" s="78" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A6</f>
         <v>SPI_CMD_WAIT</v>
       </c>
-      <c r="C16" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" s="66" t="n">
-        <v>7</v>
-      </c>
-      <c r="E16" s="66"/>
-      <c r="F16" s="81" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="75" t="s">
-        <v>299</v>
-      </c>
-      <c r="B17" s="66"/>
-      <c r="C17" s="66"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="76" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="77" t="s">
-        <v>278</v>
-      </c>
-      <c r="B18" s="78" t="str">
-        <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A6</f>
-        <v>SPI_CMD_WAIT</v>
-      </c>
-      <c r="C18" s="78" t="n">
+      <c r="C17" s="78" t="n">
         <v>28</v>
       </c>
-      <c r="D18" s="78" t="n">
+      <c r="D17" s="78" t="n">
         <v>4</v>
       </c>
-      <c r="E18" s="78" t="str">
+      <c r="E17" s="78" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!C6</f>
         <v>0x5</v>
       </c>
-      <c r="F18" s="79" t="s">
+      <c r="F17" s="79" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="72" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="72" t="s">
-        <v>302</v>
-      </c>
-      <c r="B19" s="73" t="str">
+      <c r="B18" s="73" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A7</f>
         <v>SPI_CMD_TX_DATA</v>
       </c>
-      <c r="C19" s="73" t="n">
+      <c r="C18" s="73" t="n">
         <v>0</v>
       </c>
-      <c r="D19" s="73" t="n">
+      <c r="D18" s="73" t="n">
         <v>16</v>
       </c>
-      <c r="E19" s="82"/>
-      <c r="F19" s="74" t="s">
+      <c r="E18" s="82" t="s">
+        <v>273</v>
+      </c>
+      <c r="F18" s="74" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="75" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="83" t="str">
+        <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A7</f>
+        <v>SPI_CMD_TX_DATA</v>
+      </c>
+      <c r="C19" s="66" t="n">
+        <v>16</v>
+      </c>
+      <c r="D19" s="66" t="n">
+        <v>5</v>
+      </c>
+      <c r="E19" s="69" t="s">
+        <v>273</v>
+      </c>
+      <c r="F19" s="81" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="75" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B20" s="83" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A7</f>
         <v>SPI_CMD_TX_DATA</v>
       </c>
       <c r="C20" s="66" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D20" s="66" t="n">
-        <v>5</v>
-      </c>
-      <c r="E20" s="69"/>
-      <c r="F20" s="81" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2</v>
+      </c>
+      <c r="E20" s="69" t="s">
+        <v>273</v>
+      </c>
+      <c r="F20" s="76" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="75" t="s">
-        <v>306</v>
-      </c>
-      <c r="B21" s="83" t="str">
+        <v>288</v>
+      </c>
+      <c r="B21" s="44" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A7</f>
         <v>SPI_CMD_TX_DATA</v>
       </c>
-      <c r="C21" s="66" t="n">
-        <v>21</v>
-      </c>
-      <c r="D21" s="66" t="n">
-        <v>2</v>
-      </c>
-      <c r="E21" s="69"/>
-      <c r="F21" s="76" t="s">
-        <v>307</v>
+      <c r="C21" s="44" t="n">
+        <v>26</v>
+      </c>
+      <c r="D21" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" s="46" t="s">
+        <v>273</v>
+      </c>
+      <c r="F21" s="81" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="75" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B22" s="44" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A7</f>
         <v>SPI_CMD_TX_DATA</v>
       </c>
-      <c r="C22" s="44" t="n">
-        <v>26</v>
-      </c>
-      <c r="D22" s="44" t="n">
+      <c r="C22" s="46" t="n">
+        <v>27</v>
+      </c>
+      <c r="D22" s="66" t="n">
         <v>1</v>
       </c>
-      <c r="E22" s="0"/>
+      <c r="E22" s="66" t="s">
+        <v>273</v>
+      </c>
       <c r="F22" s="81" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="75" t="s">
-        <v>289</v>
-      </c>
-      <c r="B23" s="44" t="str">
+      <c r="A23" s="77" t="s">
+        <v>279</v>
+      </c>
+      <c r="B23" s="78" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A7</f>
         <v>SPI_CMD_TX_DATA</v>
       </c>
-      <c r="C23" s="46" t="n">
-        <v>27</v>
-      </c>
-      <c r="D23" s="66" t="n">
-        <v>1</v>
-      </c>
-      <c r="E23" s="66"/>
-      <c r="F23" s="81" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="77" t="s">
-        <v>278</v>
-      </c>
-      <c r="B24" s="78" t="str">
-        <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A7</f>
-        <v>SPI_CMD_TX_DATA</v>
-      </c>
-      <c r="C24" s="78" t="n">
+      <c r="C23" s="78" t="n">
         <v>28</v>
       </c>
-      <c r="D24" s="78" t="n">
+      <c r="D23" s="78" t="n">
         <v>4</v>
       </c>
-      <c r="E24" s="78" t="str">
+      <c r="E23" s="78" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!C7</f>
         <v>0x6</v>
       </c>
-      <c r="F24" s="79" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="72" t="s">
-        <v>302</v>
-      </c>
-      <c r="B25" s="73" t="str">
+      <c r="F23" s="79" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="72" t="s">
+        <v>301</v>
+      </c>
+      <c r="B24" s="73" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A8</f>
         <v>SPI_CMD_RX_DATA</v>
       </c>
-      <c r="C25" s="73" t="n">
+      <c r="C24" s="73" t="n">
         <v>0</v>
       </c>
-      <c r="D25" s="73" t="n">
+      <c r="D24" s="73" t="n">
         <v>16</v>
       </c>
-      <c r="E25" s="82"/>
-      <c r="F25" s="74" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E24" s="82" t="s">
+        <v>273</v>
+      </c>
+      <c r="F24" s="74" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="75" t="s">
+        <v>303</v>
+      </c>
+      <c r="B25" s="83" t="str">
+        <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A8</f>
+        <v>SPI_CMD_RX_DATA</v>
+      </c>
+      <c r="C25" s="66" t="n">
+        <v>16</v>
+      </c>
+      <c r="D25" s="66" t="n">
+        <v>5</v>
+      </c>
+      <c r="E25" s="69" t="s">
+        <v>273</v>
+      </c>
+      <c r="F25" s="81" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="75" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B26" s="83" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A8</f>
         <v>SPI_CMD_RX_DATA</v>
       </c>
       <c r="C26" s="66" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D26" s="66" t="n">
-        <v>5</v>
-      </c>
-      <c r="E26" s="69"/>
-      <c r="F26" s="81" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2</v>
+      </c>
+      <c r="E26" s="69" t="s">
+        <v>273</v>
+      </c>
+      <c r="F26" s="76" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="75" t="s">
-        <v>306</v>
-      </c>
-      <c r="B27" s="83" t="str">
+        <v>288</v>
+      </c>
+      <c r="B27" s="44" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A8</f>
         <v>SPI_CMD_RX_DATA</v>
       </c>
-      <c r="C27" s="66" t="n">
-        <v>21</v>
-      </c>
-      <c r="D27" s="66" t="n">
-        <v>2</v>
-      </c>
-      <c r="E27" s="69"/>
-      <c r="F27" s="76" t="s">
-        <v>310</v>
+      <c r="C27" s="44" t="n">
+        <v>26</v>
+      </c>
+      <c r="D27" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" s="46" t="s">
+        <v>273</v>
+      </c>
+      <c r="F27" s="81" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="75" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B28" s="44" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A8</f>
         <v>SPI_CMD_RX_DATA</v>
       </c>
-      <c r="C28" s="44" t="n">
-        <v>26</v>
-      </c>
-      <c r="D28" s="44" t="n">
+      <c r="C28" s="46" t="n">
+        <v>27</v>
+      </c>
+      <c r="D28" s="66" t="n">
         <v>1</v>
       </c>
-      <c r="E28" s="0"/>
+      <c r="E28" s="66" t="s">
+        <v>273</v>
+      </c>
       <c r="F28" s="81" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="75" t="s">
-        <v>289</v>
-      </c>
-      <c r="B29" s="44" t="str">
+      <c r="A29" s="77" t="s">
+        <v>279</v>
+      </c>
+      <c r="B29" s="78" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A8</f>
         <v>SPI_CMD_RX_DATA</v>
       </c>
-      <c r="C29" s="46" t="n">
-        <v>27</v>
-      </c>
-      <c r="D29" s="66" t="n">
-        <v>1</v>
-      </c>
-      <c r="E29" s="66"/>
-      <c r="F29" s="81" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="77" t="s">
-        <v>278</v>
-      </c>
-      <c r="B30" s="78" t="str">
-        <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A8</f>
-        <v>SPI_CMD_RX_DATA</v>
-      </c>
-      <c r="C30" s="78" t="n">
+      <c r="C29" s="78" t="n">
         <v>28</v>
       </c>
-      <c r="D30" s="78" t="n">
+      <c r="D29" s="78" t="n">
         <v>4</v>
       </c>
-      <c r="E30" s="78" t="str">
+      <c r="E29" s="78" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!C8</f>
         <v>0x7</v>
       </c>
-      <c r="F30" s="79" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="72" t="s">
-        <v>311</v>
-      </c>
-      <c r="B31" s="73" t="str">
+      <c r="F29" s="79" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="72" t="s">
+        <v>310</v>
+      </c>
+      <c r="B30" s="73" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A9</f>
         <v>SPI_CMD_RPT</v>
       </c>
-      <c r="C31" s="73" t="n">
+      <c r="C30" s="73" t="n">
         <v>0</v>
       </c>
-      <c r="D31" s="73" t="n">
+      <c r="D30" s="73" t="n">
         <v>16</v>
       </c>
-      <c r="E31" s="73"/>
-      <c r="F31" s="74" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="77" t="s">
-        <v>278</v>
-      </c>
-      <c r="B32" s="84" t="str">
+      <c r="E30" s="73" t="s">
+        <v>273</v>
+      </c>
+      <c r="F30" s="74" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="77" t="s">
+        <v>279</v>
+      </c>
+      <c r="B31" s="84" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A9</f>
         <v>SPI_CMD_RPT</v>
       </c>
-      <c r="C32" s="84" t="n">
+      <c r="C31" s="84" t="n">
         <v>28</v>
       </c>
-      <c r="D32" s="84" t="n">
+      <c r="D31" s="84" t="n">
         <v>4</v>
       </c>
-      <c r="E32" s="84" t="str">
+      <c r="E31" s="84" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!C9</f>
         <v>0x8</v>
       </c>
-      <c r="F32" s="79" t="s">
+      <c r="F31" s="79" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="72" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="72" t="s">
-        <v>314</v>
-      </c>
-      <c r="B33" s="85" t="str">
+      <c r="B32" s="85" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A10</f>
         <v>SPI_CMD_EOT</v>
       </c>
-      <c r="C33" s="85" t="n">
+      <c r="C32" s="85" t="n">
         <v>0</v>
       </c>
-      <c r="D33" s="85" t="n">
+      <c r="D32" s="85" t="n">
         <v>1</v>
       </c>
-      <c r="E33" s="85"/>
-      <c r="F33" s="80" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="77" t="s">
-        <v>278</v>
-      </c>
-      <c r="B34" s="84" t="str">
+      <c r="E32" s="85" t="s">
+        <v>273</v>
+      </c>
+      <c r="F32" s="80" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="77" t="s">
+        <v>279</v>
+      </c>
+      <c r="B33" s="84" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A10</f>
         <v>SPI_CMD_EOT</v>
       </c>
-      <c r="C34" s="84" t="n">
+      <c r="C33" s="84" t="n">
         <v>28</v>
       </c>
-      <c r="D34" s="84" t="n">
+      <c r="D33" s="84" t="n">
         <v>4</v>
       </c>
-      <c r="E34" s="84" t="str">
+      <c r="E33" s="84" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!C10</f>
         <v>0x9</v>
       </c>
-      <c r="F34" s="79" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="86" t="s">
-        <v>278</v>
-      </c>
-      <c r="B35" s="87" t="str">
+      <c r="F33" s="79" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="86" t="s">
+        <v>279</v>
+      </c>
+      <c r="B34" s="87" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A11</f>
         <v>SPI_CMD_RPT_END</v>
       </c>
-      <c r="C35" s="87" t="n">
+      <c r="C34" s="87" t="n">
         <v>28</v>
       </c>
-      <c r="D35" s="87" t="n">
+      <c r="D34" s="87" t="n">
         <v>4</v>
       </c>
-      <c r="E35" s="87" t="str">
+      <c r="E34" s="87" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!C11</f>
         <v>0xA</v>
       </c>
-      <c r="F35" s="88" t="s">
+      <c r="F34" s="88" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="89" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="89" t="s">
-        <v>318</v>
-      </c>
-      <c r="B36" s="85" t="str">
+      <c r="B35" s="85" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A12</f>
         <v>SPI_CMD_RX_CHECK</v>
       </c>
-      <c r="C36" s="85" t="n">
+      <c r="C35" s="85" t="n">
         <v>0</v>
       </c>
-      <c r="D36" s="85" t="n">
+      <c r="D35" s="85" t="n">
         <v>16</v>
       </c>
-      <c r="E36" s="85"/>
-      <c r="F36" s="74" t="s">
+      <c r="E35" s="85" t="s">
+        <v>273</v>
+      </c>
+      <c r="F35" s="74" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="90" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="44" t="str">
+        <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A12</f>
+        <v>SPI_CMD_RX_CHECK</v>
+      </c>
+      <c r="C36" s="44" t="n">
+        <v>16</v>
+      </c>
+      <c r="D36" s="44" t="n">
+        <v>4</v>
+      </c>
+      <c r="E36" s="46" t="s">
+        <v>273</v>
+      </c>
+      <c r="F36" s="81" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="43.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="90" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B37" s="44" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A12</f>
         <v>SPI_CMD_RX_CHECK</v>
       </c>
       <c r="C37" s="44" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D37" s="44" t="n">
-        <v>4</v>
-      </c>
-      <c r="E37" s="0"/>
-      <c r="F37" s="81" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="90" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" s="46" t="s">
+        <v>273</v>
+      </c>
+      <c r="F37" s="76" t="s">
         <v>322</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="75" t="s">
+        <v>288</v>
       </c>
       <c r="B38" s="44" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A12</f>
         <v>SPI_CMD_RX_CHECK</v>
       </c>
       <c r="C38" s="44" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D38" s="44" t="n">
-        <v>2</v>
-      </c>
-      <c r="E38" s="0"/>
-      <c r="F38" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" s="46" t="s">
+        <v>273</v>
+      </c>
+      <c r="F38" s="81" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="75" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="B39" s="44" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A12</f>
         <v>SPI_CMD_RX_CHECK</v>
       </c>
-      <c r="C39" s="44" t="n">
-        <v>26</v>
-      </c>
-      <c r="D39" s="44" t="n">
+      <c r="C39" s="46" t="n">
+        <v>27</v>
+      </c>
+      <c r="D39" s="66" t="n">
         <v>1</v>
       </c>
-      <c r="E39" s="0"/>
+      <c r="E39" s="66" t="s">
+        <v>273</v>
+      </c>
       <c r="F39" s="81" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="75" t="s">
-        <v>289</v>
-      </c>
-      <c r="B40" s="44" t="str">
+      <c r="A40" s="77" t="s">
+        <v>279</v>
+      </c>
+      <c r="B40" s="84" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A12</f>
         <v>SPI_CMD_RX_CHECK</v>
       </c>
-      <c r="C40" s="46" t="n">
-        <v>27</v>
-      </c>
-      <c r="D40" s="66" t="n">
-        <v>1</v>
-      </c>
-      <c r="E40" s="66"/>
-      <c r="F40" s="81" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="77" t="s">
-        <v>278</v>
-      </c>
-      <c r="B41" s="84" t="str">
-        <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A12</f>
-        <v>SPI_CMD_RX_CHECK</v>
-      </c>
-      <c r="C41" s="84" t="n">
+      <c r="C40" s="84" t="n">
         <v>28</v>
       </c>
-      <c r="D41" s="84" t="n">
+      <c r="D40" s="84" t="n">
         <v>4</v>
       </c>
-      <c r="E41" s="84" t="str">
+      <c r="E40" s="84" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!C12</f>
         <v>0xB</v>
       </c>
-      <c r="F41" s="79" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="72" t="s">
-        <v>285</v>
-      </c>
-      <c r="B42" s="85" t="str">
+      <c r="F40" s="79" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="72" t="s">
+        <v>286</v>
+      </c>
+      <c r="B41" s="85" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A13</f>
         <v>SPI_CMD_FULL_DUPL</v>
       </c>
-      <c r="C42" s="73" t="n">
+      <c r="C41" s="73" t="n">
         <v>0</v>
       </c>
-      <c r="D42" s="73" t="n">
+      <c r="D41" s="73" t="n">
         <v>16</v>
       </c>
-      <c r="E42" s="85"/>
-      <c r="F42" s="74" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="75" t="s">
-        <v>287</v>
-      </c>
-      <c r="B43" s="44" t="str">
+      <c r="E41" s="85" t="s">
+        <v>273</v>
+      </c>
+      <c r="F41" s="74" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="75" t="s">
+        <v>288</v>
+      </c>
+      <c r="B42" s="44" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A13</f>
         <v>SPI_CMD_FULL_DUPL</v>
       </c>
-      <c r="C43" s="44" t="n">
+      <c r="C42" s="44" t="n">
         <v>26</v>
       </c>
-      <c r="D43" s="44" t="n">
+      <c r="D42" s="44" t="n">
         <v>1</v>
       </c>
-      <c r="E43" s="0"/>
-      <c r="F43" s="81" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="77" t="s">
-        <v>278</v>
-      </c>
-      <c r="B44" s="84" t="str">
+      <c r="E42" s="46" t="s">
+        <v>273</v>
+      </c>
+      <c r="F42" s="81" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="77" t="s">
+        <v>279</v>
+      </c>
+      <c r="B43" s="84" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A13</f>
         <v>SPI_CMD_FULL_DUPL</v>
       </c>
-      <c r="C44" s="84" t="n">
+      <c r="C43" s="84" t="n">
         <v>28</v>
       </c>
-      <c r="D44" s="84" t="n">
+      <c r="D43" s="84" t="n">
         <v>4</v>
       </c>
-      <c r="E44" s="84" t="str">
+      <c r="E43" s="84" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!C13</f>
         <v>0xC</v>
       </c>
-      <c r="F44" s="79" t="s">
+      <c r="F43" s="79" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="72" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="72" t="s">
-        <v>329</v>
-      </c>
-      <c r="B45" s="85" t="str">
+      <c r="B44" s="85" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A14</f>
         <v>SPI_CMD_SETUP_UCA</v>
       </c>
-      <c r="C45" s="85" t="n">
+      <c r="C44" s="85" t="n">
         <v>0</v>
       </c>
-      <c r="D45" s="85" t="s">
-        <v>330</v>
-      </c>
-      <c r="E45" s="85"/>
-      <c r="F45" s="74" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="77" t="s">
-        <v>278</v>
-      </c>
-      <c r="B46" s="84" t="str">
+      <c r="D44" s="85" t="n">
+        <v>21</v>
+      </c>
+      <c r="E44" s="85" t="s">
+        <v>273</v>
+      </c>
+      <c r="F44" s="74" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="77" t="s">
+        <v>279</v>
+      </c>
+      <c r="B45" s="84" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A14</f>
         <v>SPI_CMD_SETUP_UCA</v>
       </c>
-      <c r="C46" s="84" t="n">
+      <c r="C45" s="84" t="n">
         <v>28</v>
       </c>
-      <c r="D46" s="84" t="n">
+      <c r="D45" s="84" t="n">
         <v>4</v>
       </c>
-      <c r="E46" s="84" t="str">
+      <c r="E45" s="84" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!C14</f>
         <v>0xD</v>
       </c>
-      <c r="F46" s="79" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="72"/>
-      <c r="B47" s="85" t="str">
+      <c r="F45" s="79" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="72" t="s">
+        <v>331</v>
+      </c>
+      <c r="B46" s="85" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A15</f>
         <v>SPI_CMD_SETUP_UCS</v>
       </c>
-      <c r="C47" s="85"/>
-      <c r="D47" s="85" t="s">
+      <c r="C46" s="85" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" s="85" t="n">
+        <v>20</v>
+      </c>
+      <c r="E46" s="85" t="s">
+        <v>273</v>
+      </c>
+      <c r="F46" s="74" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="43.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="75" t="s">
+        <v>305</v>
+      </c>
+      <c r="B47" s="44" t="str">
+        <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A15</f>
+        <v>SPI_CMD_SETUP_UCS</v>
+      </c>
+      <c r="C47" s="44" t="n">
+        <v>25</v>
+      </c>
+      <c r="D47" s="44" t="n">
+        <v>2</v>
+      </c>
+      <c r="E47" s="46" t="s">
+        <v>273</v>
+      </c>
+      <c r="F47" s="76" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="75" t="s">
         <v>333</v>
-      </c>
-      <c r="E47" s="85"/>
-      <c r="F47" s="74" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="75" t="s">
-        <v>306</v>
       </c>
       <c r="B48" s="44" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A15</f>
         <v>SPI_CMD_SETUP_UCS</v>
       </c>
       <c r="C48" s="44" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D48" s="44" t="n">
-        <v>2</v>
-      </c>
-      <c r="E48" s="0"/>
+        <v>1</v>
+      </c>
+      <c r="E48" s="46" t="s">
+        <v>273</v>
+      </c>
       <c r="F48" s="76" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="75" t="s">
-        <v>335</v>
-      </c>
-      <c r="B49" s="44" t="str">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="77" t="s">
+        <v>279</v>
+      </c>
+      <c r="B49" s="84" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A15</f>
         <v>SPI_CMD_SETUP_UCS</v>
       </c>
-      <c r="C49" s="44" t="n">
-        <v>27</v>
-      </c>
-      <c r="D49" s="44" t="n">
-        <v>1</v>
-      </c>
-      <c r="E49" s="0"/>
-      <c r="F49" s="76" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="77" t="s">
-        <v>278</v>
-      </c>
-      <c r="B50" s="84" t="str">
-        <f aca="false">'IPUDMACMDLIST_rel1.0.0'!A15</f>
-        <v>SPI_CMD_SETUP_UCS</v>
-      </c>
-      <c r="C50" s="84" t="n">
+      <c r="C49" s="84" t="n">
         <v>28</v>
       </c>
-      <c r="D50" s="84" t="n">
+      <c r="D49" s="84" t="n">
         <v>4</v>
       </c>
-      <c r="E50" s="84" t="str">
+      <c r="E49" s="84" t="str">
         <f aca="false">'IPUDMACMDLIST_rel1.0.0'!C15</f>
         <v>0xE</v>
       </c>
-      <c r="F50" s="79" t="s">
-        <v>337</v>
+      <c r="F49" s="79" t="s">
+        <v>335</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>